<commit_message>
template was edited: 20 (4x5) stickers per page
</commit_message>
<xml_diff>
--- a/Templates/template.xlsx
+++ b/Templates/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROGRAMMING\EnglishWordsToPrint\bin\Debug\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROGRAMMING\EnglishWordsPrintUtility\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603C8B7F-243B-423C-8FAC-92C5035B45AD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C886EF90-D698-4DE9-A63C-C9187DC13AFD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="0" windowWidth="20490" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,16 +18,17 @@
     <sheet name="#dynamic" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="__Pages__X">Sheet1!$A$1:$P$42</definedName>
-    <definedName name="__Stickers__X">Sheet1!$A$1:$D$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$3:$P$43</definedName>
+    <definedName name="__Pages__X">Sheet1!$A$1:$P$36</definedName>
+    <definedName name="__Stickers__X">Sheet1!$A$1:$P$7</definedName>
+    <definedName name="keeprows_1_a">Sheet1!$A$1:$P$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$36</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Source Name</t>
   </si>
@@ -103,21 +104,23 @@
   </si>
   <si>
     <t>&lt;#Stickers.Russian&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#auto page breaks&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy\ h:mm;@"/>
-    <numFmt numFmtId="167" formatCode="[ss]"/>
-    <numFmt numFmtId="168" formatCode="&quot;A -&quot;\ 0.00000"/>
-    <numFmt numFmtId="169" formatCode="&quot;B +&quot;\ 0.00000"/>
+    <numFmt numFmtId="166" formatCode="[ss]"/>
+    <numFmt numFmtId="167" formatCode="&quot;A -&quot;\ 0.00000"/>
+    <numFmt numFmtId="168" formatCode="&quot;B +&quot;\ 0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,20 +165,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
+      <i/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
-      <i/>
-      <sz val="14"/>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -389,30 +400,50 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -431,24 +462,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -802,24 +815,13 @@
   </sheetPr>
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection sqref="A1:P36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13" style="9" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="9" customWidth="1"/>
-    <col min="5" max="6" width="12.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="9" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="9"/>
-    <col min="10" max="10" width="12.42578125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="9" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="9"/>
-    <col min="14" max="14" width="9.140625" style="9" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="16384" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -829,30 +831,63 @@
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
       <c r="D1" s="35"/>
+      <c r="E1" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="35"/>
+      <c r="R1" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
       <c r="D2" s="38"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="38"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="38"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="38"/>
       <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -860,34 +895,36 @@
       <c r="B4" s="37"/>
       <c r="C4" s="37"/>
       <c r="D4" s="38"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="38"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="39"/>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
       <c r="D5" s="41"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="41"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
     </row>
@@ -898,18 +935,24 @@
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="44"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="E6" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="44"/>
       <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -917,50 +960,50 @@
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
       <c r="D7" s="47"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="47"/>
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
@@ -1359,12 +1402,19 @@
       <c r="M44" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
+    <mergeCell ref="M1:P5"/>
+    <mergeCell ref="M6:P7"/>
     <mergeCell ref="A6:D7"/>
     <mergeCell ref="A1:D5"/>
+    <mergeCell ref="E1:H5"/>
+    <mergeCell ref="E6:H7"/>
+    <mergeCell ref="I1:L5"/>
+    <mergeCell ref="I6:L7"/>
   </mergeCells>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0" bottom="0.74803149606299213" header="0" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="87" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
The models reworked according with template 4 stickers per row
</commit_message>
<xml_diff>
--- a/Templates/template.xlsx
+++ b/Templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROGRAMMING\EnglishWordsPrintUtility\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C886EF90-D698-4DE9-A63C-C9187DC13AFD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF15CE17-B8E3-412D-A85F-AAED734CAABB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="0" windowWidth="20490" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="__Pages__X">Sheet1!$A$1:$P$36</definedName>
-    <definedName name="__Stickers__X">Sheet1!$A$1:$P$7</definedName>
+    <definedName name="__Rows__X">Sheet1!$A$1:$P$7</definedName>
     <definedName name="keeprows_1_a">Sheet1!$A$1:$P$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$36</definedName>
   </definedNames>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Source Name</t>
   </si>
@@ -100,13 +100,31 @@
     <t>&lt;#if(&lt;#FromLaserFrequency&gt;;( &lt;#evaluate(round(&lt;#FromLaserFrequency&gt;,2))&gt; nm );&lt;#ActualOrNominalWavelength(&lt;#Actual&gt;;&lt;#Nominal&gt;)&gt; nm)&gt;</t>
   </si>
   <si>
-    <t>&lt;#Stickers.English&gt;</t>
-  </si>
-  <si>
-    <t>&lt;#Stickers.Russian&gt;</t>
-  </si>
-  <si>
     <t>&lt;#auto page breaks&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column1.English&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column1.Russian&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column2.English&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column2.Russian&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column3.English&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column3.Russian&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column4.English&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column4.Russian&gt;</t>
   </si>
 </sst>
 </file>
@@ -816,7 +834,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection sqref="A1:P36"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -826,31 +844,31 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
       <c r="D1" s="35"/>
       <c r="E1" s="33" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
       <c r="H1" s="35"/>
       <c r="I1" s="33" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J1" s="34"/>
       <c r="K1" s="34"/>
       <c r="L1" s="35"/>
       <c r="M1" s="33" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="N1" s="34"/>
       <c r="O1" s="34"/>
       <c r="P1" s="35"/>
       <c r="R1" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -930,25 +948,25 @@
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="44"/>
       <c r="E6" s="42" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
       <c r="H6" s="44"/>
       <c r="I6" s="42" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J6" s="43"/>
       <c r="K6" s="43"/>
       <c r="L6" s="44"/>
       <c r="M6" s="42" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="N6" s="43"/>
       <c r="O6" s="43"/>

</xml_diff>

<commit_message>
used wooordhunt to get spelling and russian
</commit_message>
<xml_diff>
--- a/Templates/template.xlsx
+++ b/Templates/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROGRAMMING\EnglishWordsPrintUtility\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9098E946-E6F1-4C0D-AB1C-01D9023E736B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101DB74A-2571-46E2-BB83-0FF7488C351B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="0" windowWidth="20490" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Source Name</t>
   </si>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>&lt;#Rows.Column4.Russian&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column1.Spell&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column2.Spell&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column3.Spell&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#Rows.Column4.Spell&gt;</t>
   </si>
 </sst>
 </file>
@@ -200,7 +212,7 @@
     </font>
     <font>
       <i/>
-      <sz val="12"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -377,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -437,6 +449,12 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,42 +467,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный_&lt;#CONFIG&gt;" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -508,9 +511,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -548,7 +551,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -654,7 +657,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -834,7 +837,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="M1" sqref="M1:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -842,154 +845,162 @@
     <col min="1" max="16384" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="33" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="33" t="s">
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="33" t="s">
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="37"/>
       <c r="R1" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="38"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="38"/>
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="39"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="39"/>
       <c r="Q3" s="10"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="38"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="39"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="41"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="E5" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="41"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
+      <c r="I5" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
       <c r="L5" s="41"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
+      <c r="M5" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
       <c r="P5" s="41"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="44"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="41"/>
       <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="47"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="44"/>
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1420,15 +1431,19 @@
       <c r="M44" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="M1:P5"/>
-    <mergeCell ref="M6:P7"/>
-    <mergeCell ref="A6:D7"/>
-    <mergeCell ref="A1:D5"/>
-    <mergeCell ref="E1:H5"/>
-    <mergeCell ref="E6:H7"/>
-    <mergeCell ref="I1:L5"/>
-    <mergeCell ref="I6:L7"/>
+  <mergeCells count="12">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="A5:D7"/>
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="E5:H7"/>
+    <mergeCell ref="I5:L7"/>
+    <mergeCell ref="M5:P7"/>
+    <mergeCell ref="I1:L2"/>
+    <mergeCell ref="M1:P2"/>
+    <mergeCell ref="E3:H4"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="M3:P4"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Refactoring. Added supporting highlighted cells in gsheets. Refused using csv as words repository. Template edited: made spell italic, foreground gray, made rus 12 fontsize
</commit_message>
<xml_diff>
--- a/Templates/template.xlsx
+++ b/Templates/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROGRAMMING\EnglishWordsPrintUtility\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work for myself\EnglishWordsPrintUtility\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101DB74A-2571-46E2-BB83-0FF7488C351B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB826B2-E7D7-47AF-9BD2-E3A817AE03F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>Source Name</t>
   </si>
@@ -150,7 +150,7 @@
     <numFmt numFmtId="167" formatCode="&quot;A -&quot;\ 0.00000"/>
     <numFmt numFmtId="168" formatCode="&quot;B +&quot;\ 0.00000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,8 +212,17 @@
     </font>
     <font>
       <i/>
-      <sz val="8"/>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -389,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -449,30 +458,12 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -484,6 +475,33 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -837,7 +855,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P7"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -846,161 +864,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="35" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="35" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="35" t="s">
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="37"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="41"/>
       <c r="R1" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="39"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="44"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="38" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="38" t="s">
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="38" t="s">
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="39"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="47"/>
       <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="39"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="47"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="40" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="40" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="40" t="s">
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="41"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="35"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="41"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="35"/>
       <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="44"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="38"/>
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>